<commit_message>
Added new excel sheet with updated data which was causing fail login with valid cred TC
</commit_message>
<xml_diff>
--- a/src/main/resources/testData/TutorialsNinjaCred.xlsx
+++ b/src/main/resources/testData/TutorialsNinjaCred.xlsx
@@ -3,9 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{9499B86F-C838-45A2-BB83-EED6A6BD3D7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\TestData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE8C5978-855E-439F-A1D1-960B6542A053}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="emp" sheetId="1" r:id="rId1"/>
@@ -14,8 +19,7 @@
     <sheet name="dataProvider" sheetId="4" r:id="rId4"/>
     <sheet name="registerCred" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="0"/>
-  <oleSize ref="A1:L12"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -165,9 +169,6 @@
     <t>Pixel@1954</t>
   </si>
   <si>
-    <t>Pixel@1955</t>
-  </si>
-  <si>
     <t>fName</t>
   </si>
   <si>
@@ -190,6 +191,9 @@
   </si>
   <si>
     <t>Nande</t>
+  </si>
+  <si>
+    <t>Pixel@1953</t>
   </si>
 </sst>
 </file>
@@ -883,8 +887,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AD529B1-EC1D-4479-8BAD-8449CCDB0F9F}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -914,7 +918,7 @@
         <v>43</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -941,7 +945,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E810F993-4F86-4135-ADA0-9D091B9E6C1E}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -953,34 +957,34 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>47</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>